<commit_message>
Updated tm52_calc to use create_df_from_criterion
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
@@ -27,18 +27,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="129">
   <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
+    <t>JobNo</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>Author</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
-    <t>JobNo</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -72,46 +72,46 @@
     <t>10</t>
   </si>
   <si>
-    <t>O.Hensby</t>
+    <t>Project Information</t>
+  </si>
+  <si>
+    <t>Criterion % Definitions</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.15</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.2</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.3</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.4</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.5</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.6</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.7</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.8</t>
+  </si>
+  <si>
+    <t>/c/e</t>
   </si>
   <si>
     <t>20220301</t>
   </si>
   <si>
-    <t>Project Information</t>
-  </si>
-  <si>
-    <t>Criterion % Definitions</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.15</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.2</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.3</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.4</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.5</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.6</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.7</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.8</t>
-  </si>
-  <si>
-    <t>ngDe</t>
+    <t>jovyan</t>
   </si>
   <si>
     <t>index</t>
@@ -177,7 +177,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-01 13:26:31.239471</t>
+    <t>2022-03-01 21:00:04.952100</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -195,7 +195,7 @@
     <t>Criterion 3 (Max Delta T)</t>
   </si>
   <si>
-    <t>The percentage of occupied hours where delta T equals or excedes the threshold (1 kelvin) over the total occupied hours.</t>
+    <t>The percentage of occupied hours where delta T equals or exceeds the threshold (1 kelvin) over the total occupied hours.</t>
   </si>
   <si>
     <t>The maximum daily weight taken from the year.</t>
@@ -418,7 +418,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,14 +429,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -499,7 +491,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -603,10 +595,10 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="Author"/>
-    <tableColumn id="3" name="Date"/>
-    <tableColumn id="4" name="sheet_name"/>
-    <tableColumn id="5" name="JobNo"/>
+    <tableColumn id="2" name="sheet_name"/>
+    <tableColumn id="3" name="JobNo"/>
+    <tableColumn id="4" name="Date"/>
+    <tableColumn id="5" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -627,7 +619,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -646,7 +638,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -665,7 +657,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -676,7 +668,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Information"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -687,7 +679,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Definition"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -706,7 +698,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -725,7 +717,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -744,7 +736,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -763,7 +755,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -782,7 +774,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -801,7 +793,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1130,10 +1122,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
@@ -1144,13 +1136,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
@@ -1161,13 +1153,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -1178,13 +1170,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
@@ -1195,13 +1187,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
@@ -1212,13 +1204,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
@@ -1229,13 +1221,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
@@ -1246,13 +1238,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1263,13 +1255,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>28</v>
@@ -1280,13 +1272,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -1297,10 +1289,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
@@ -7278,7 +7270,7 @@
         <v>112</v>
       </c>
       <c r="D18">
-        <v>8.2</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E18" t="s">
         <v>128</v>
@@ -7342,7 +7334,7 @@
         <v>114</v>
       </c>
       <c r="D20">
-        <v>8.2</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E20" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
Updated deltaT calc to accommodate for different max acceptable temperatures depending on category
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
@@ -27,18 +27,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="129">
   <si>
+    <t>JobNo</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
     <t>sheet_name</t>
   </si>
   <si>
-    <t>JobNo</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -72,6 +72,15 @@
     <t>10</t>
   </si>
   <si>
+    <t>ngDe</t>
+  </si>
+  <si>
+    <t>20220302</t>
+  </si>
+  <si>
+    <t>O.Hensby</t>
+  </si>
+  <si>
     <t>Project Information</t>
   </si>
   <si>
@@ -105,15 +114,6 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>/c/e</t>
-  </si>
-  <si>
-    <t>20220301</t>
-  </si>
-  <si>
-    <t>jovyan</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -177,7 +177,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-01 21:00:04.952100</t>
+    <t>2022-03-02 15:11:42.399175</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -195,7 +195,7 @@
     <t>Criterion 3 (Max Delta T)</t>
   </si>
   <si>
-    <t>The percentage of occupied hours where delta T equals or exceeds the threshold (1 kelvin) over the total occupied hours.</t>
+    <t>The percentage of occupied hours where delta T equals or excedes the threshold (1 kelvin) over the total occupied hours.</t>
   </si>
   <si>
     <t>The maximum daily weight taken from the year.</t>
@@ -418,7 +418,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +429,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -491,7 +499,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -595,10 +603,10 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="sheet_name"/>
-    <tableColumn id="3" name="JobNo"/>
-    <tableColumn id="4" name="Date"/>
-    <tableColumn id="5" name="Author"/>
+    <tableColumn id="2" name="JobNo"/>
+    <tableColumn id="3" name="Date"/>
+    <tableColumn id="4" name="Author"/>
+    <tableColumn id="5" name="sheet_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -619,7 +627,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -638,7 +646,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -657,7 +665,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -668,7 +676,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Information"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -679,7 +687,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Definition"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -698,7 +706,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -717,7 +725,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -736,7 +744,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -755,7 +763,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -774,7 +782,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -793,7 +801,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1122,13 +1130,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1136,16 +1144,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1153,16 +1161,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1170,16 +1178,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1187,16 +1195,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1204,16 +1212,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1221,16 +1229,16 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1238,16 +1246,16 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1255,16 +1263,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1272,16 +1280,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1289,13 +1297,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
@@ -7270,7 +7278,7 @@
         <v>112</v>
       </c>
       <c r="D18">
-        <v>8.199999999999999</v>
+        <v>8.2</v>
       </c>
       <c r="E18" t="s">
         <v>128</v>
@@ -7334,7 +7342,7 @@
         <v>114</v>
       </c>
       <c r="D20">
-        <v>8.199999999999999</v>
+        <v>8.2</v>
       </c>
       <c r="E20" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
Removed print statements from tm59 calc
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
     <sheet name="Project Information" sheetId="2" r:id="rId2"/>
-    <sheet name="Criterion % Definitions" sheetId="3" r:id="rId3"/>
+    <sheet name="Criterion Definitions" sheetId="3" r:id="rId3"/>
     <sheet name="Results, Air Speed 0.1" sheetId="4" r:id="rId4"/>
     <sheet name="Results, Air Speed 0.15" sheetId="5" r:id="rId5"/>
     <sheet name="Results, Air Speed 0.2" sheetId="6" r:id="rId6"/>
@@ -30,15 +30,15 @@
     <t>JobNo</t>
   </si>
   <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
     <t>Author</t>
   </si>
   <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -75,45 +75,45 @@
     <t>ngDe</t>
   </si>
   <si>
+    <t>Project Information</t>
+  </si>
+  <si>
+    <t>Criterion Definitions</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.15</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.2</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.3</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.4</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.5</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.6</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.7</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.8</t>
+  </si>
+  <si>
     <t>20220302</t>
   </si>
   <si>
     <t>O.Hensby</t>
   </si>
   <si>
-    <t>Project Information</t>
-  </si>
-  <si>
-    <t>Criterion % Definitions</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.15</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.2</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.3</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.4</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.5</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.6</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.7</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.8</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -177,7 +177,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-02 15:11:42.399175</t>
+    <t>2022-03-02 16:50:29.101876</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -195,7 +195,7 @@
     <t>Criterion 3 (Max Delta T)</t>
   </si>
   <si>
-    <t>The percentage of occupied hours where delta T equals or excedes the threshold (1 kelvin) over the total occupied hours.</t>
+    <t>The percentage of occupied hours where delta T equals or exceeds the threshold (1 kelvin) over the total occupied hours.</t>
   </si>
   <si>
     <t>The maximum daily weight taken from the year.</t>
@@ -604,9 +604,9 @@
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="JobNo"/>
-    <tableColumn id="3" name="Date"/>
-    <tableColumn id="4" name="Author"/>
-    <tableColumn id="5" name="sheet_name"/>
+    <tableColumn id="3" name="sheet_name"/>
+    <tableColumn id="4" name="Date"/>
+    <tableColumn id="5" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1133,10 +1133,10 @@
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1147,13 +1147,13 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1164,13 +1164,13 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1181,13 +1181,13 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1198,13 +1198,13 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1215,13 +1215,13 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1232,13 +1232,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1249,13 +1249,13 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1266,13 +1266,13 @@
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1283,13 +1283,13 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1300,10 +1300,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
separated mechvent from tm59 folder
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
@@ -30,15 +30,15 @@
     <t>Author</t>
   </si>
   <si>
+    <t>JobNo</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>sheet_name</t>
   </si>
   <si>
-    <t>JobNo</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -72,7 +72,13 @@
     <t>10</t>
   </si>
   <si>
-    <t>jovyan</t>
+    <t>O.Hensby</t>
+  </si>
+  <si>
+    <t>ngDe</t>
+  </si>
+  <si>
+    <t>20220303</t>
   </si>
   <si>
     <t>Project Information</t>
@@ -108,12 +114,6 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>/c/e</t>
-  </si>
-  <si>
-    <t>20220302</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -177,7 +177,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-02 17:12:56.537527</t>
+    <t>2022-03-03 15:15:39.409239</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -418,7 +418,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +429,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -491,7 +499,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -596,9 +604,9 @@
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Author"/>
-    <tableColumn id="3" name="sheet_name"/>
-    <tableColumn id="4" name="JobNo"/>
-    <tableColumn id="5" name="Date"/>
+    <tableColumn id="3" name="JobNo"/>
+    <tableColumn id="4" name="Date"/>
+    <tableColumn id="5" name="sheet_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -619,7 +627,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -638,7 +646,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -657,7 +665,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -668,7 +676,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Information"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -679,7 +687,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Definition"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -698,7 +706,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -717,7 +725,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -736,7 +744,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -755,7 +763,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -774,7 +782,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -793,7 +801,7 @@
     <tableColumn id="9" name="Criterion 3 (Pass/Fail)"/>
     <tableColumn id="10" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1125,10 +1133,10 @@
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1139,13 +1147,13 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1156,13 +1164,13 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1173,13 +1181,13 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1190,13 +1198,13 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1207,13 +1215,13 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1224,13 +1232,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1241,13 +1249,13 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1258,13 +1266,13 @@
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1275,13 +1283,13 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1292,10 +1300,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
@@ -7270,7 +7278,7 @@
         <v>112</v>
       </c>
       <c r="D18">
-        <v>8.199999999999999</v>
+        <v>8.2</v>
       </c>
       <c r="E18" t="s">
         <v>128</v>
@@ -7334,7 +7342,7 @@
         <v>114</v>
       </c>
       <c r="D20">
-        <v>8.199999999999999</v>
+        <v>8.2</v>
       </c>
       <c r="E20" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
Changed name of tm59 mech vent excel file when output
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
@@ -33,12 +33,12 @@
     <t>Date</t>
   </si>
   <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
     <t>Author</t>
   </si>
   <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -78,42 +78,42 @@
     <t>20220303</t>
   </si>
   <si>
+    <t>Project Information</t>
+  </si>
+  <si>
+    <t>Criterion Definitions</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.15</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.2</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.3</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.4</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.5</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.6</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.7</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.8</t>
+  </si>
+  <si>
     <t>O.Hensby</t>
   </si>
   <si>
-    <t>Project Information</t>
-  </si>
-  <si>
-    <t>Criterion Definitions</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.15</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.2</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.3</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.4</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.5</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.6</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.7</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.8</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -177,7 +177,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-03 15:33:43.320121</t>
+    <t>2022-03-03 16:22:36.779643</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -605,8 +605,8 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="JobNo"/>
     <tableColumn id="3" name="Date"/>
-    <tableColumn id="4" name="Author"/>
-    <tableColumn id="5" name="sheet_name"/>
+    <tableColumn id="4" name="sheet_name"/>
+    <tableColumn id="5" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1136,7 +1136,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1150,10 +1150,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1167,10 +1167,10 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1184,10 +1184,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1201,10 +1201,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1218,10 +1218,10 @@
         <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1235,10 +1235,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1252,10 +1252,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1269,10 +1269,10 @@
         <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1286,10 +1286,10 @@
         <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1303,7 +1303,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
set index to Room ID in final df
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
@@ -27,15 +27,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="129">
   <si>
+    <t>Author</t>
+  </si>
+  <si>
     <t>sheet_name</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>JobNo</t>
   </si>
   <si>
@@ -72,6 +72,9 @@
     <t>10</t>
   </si>
   <si>
+    <t>jovyan</t>
+  </si>
+  <si>
     <t>Project Information</t>
   </si>
   <si>
@@ -108,9 +111,6 @@
     <t>20220308</t>
   </si>
   <si>
-    <t>jovyan</t>
-  </si>
-  <si>
     <t>/c/e</t>
   </si>
   <si>
@@ -177,7 +177,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-08 14:44:03.338663</t>
+    <t>2022-03-08 14:52:54.463102</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -204,22 +204,115 @@
     <t>The maximum delta T taken from the year.</t>
   </si>
   <si>
+    <t>Room Name</t>
+  </si>
+  <si>
+    <t>Criterion 1 (Pass/Fail)</t>
+  </si>
+  <si>
+    <t>Criterion 2 (Pass/Fail)</t>
+  </si>
+  <si>
+    <t>Criterion 3 (Pass/Fail)</t>
+  </si>
+  <si>
+    <t>TM52 (Pass/Fail)</t>
+  </si>
+  <si>
     <t>Room ID</t>
   </si>
   <si>
-    <t>Criterion 1 (Pass/Fail)</t>
-  </si>
-  <si>
-    <t>Criterion 2 (Pass/Fail)</t>
-  </si>
-  <si>
-    <t>Criterion 3 (Pass/Fail)</t>
-  </si>
-  <si>
-    <t>TM52 (Pass/Fail)</t>
-  </si>
-  <si>
-    <t>Room Name</t>
+    <t>1S000001</t>
+  </si>
+  <si>
+    <t>1S000002</t>
+  </si>
+  <si>
+    <t>1S000003</t>
+  </si>
+  <si>
+    <t>1S000004</t>
+  </si>
+  <si>
+    <t>1S000005</t>
+  </si>
+  <si>
+    <t>1S000006</t>
+  </si>
+  <si>
+    <t>1S000007</t>
+  </si>
+  <si>
+    <t>2N000001</t>
+  </si>
+  <si>
+    <t>2N000002</t>
+  </si>
+  <si>
+    <t>2N000003</t>
+  </si>
+  <si>
+    <t>2N000004</t>
+  </si>
+  <si>
+    <t>2N000005</t>
+  </si>
+  <si>
+    <t>2N000006</t>
+  </si>
+  <si>
+    <t>2N000007</t>
+  </si>
+  <si>
+    <t>2N000008</t>
+  </si>
+  <si>
+    <t>3R000001</t>
+  </si>
+  <si>
+    <t>3R000002</t>
+  </si>
+  <si>
+    <t>3R000003</t>
+  </si>
+  <si>
+    <t>3R000004</t>
+  </si>
+  <si>
+    <t>3R000005</t>
+  </si>
+  <si>
+    <t>3R000006</t>
+  </si>
+  <si>
+    <t>3R000007</t>
+  </si>
+  <si>
+    <t>3R000008</t>
+  </si>
+  <si>
+    <t>4T000001</t>
+  </si>
+  <si>
+    <t>4T000002</t>
+  </si>
+  <si>
+    <t>4T000003</t>
+  </si>
+  <si>
+    <t>4T000004</t>
+  </si>
+  <si>
+    <t>4T000005</t>
+  </si>
+  <si>
+    <t>4T000006</t>
+  </si>
+  <si>
+    <t>4T000007</t>
+  </si>
+  <si>
+    <t>4T000008</t>
   </si>
   <si>
     <t>A_01_XX_XX_ApartmentSW</t>
@@ -313,99 +406,6 @@
   </si>
   <si>
     <t>A_04_XX_XX_ApartmentN2</t>
-  </si>
-  <si>
-    <t>1S000001</t>
-  </si>
-  <si>
-    <t>1S000002</t>
-  </si>
-  <si>
-    <t>1S000003</t>
-  </si>
-  <si>
-    <t>1S000004</t>
-  </si>
-  <si>
-    <t>1S000005</t>
-  </si>
-  <si>
-    <t>1S000006</t>
-  </si>
-  <si>
-    <t>1S000007</t>
-  </si>
-  <si>
-    <t>2N000001</t>
-  </si>
-  <si>
-    <t>2N000002</t>
-  </si>
-  <si>
-    <t>2N000003</t>
-  </si>
-  <si>
-    <t>2N000004</t>
-  </si>
-  <si>
-    <t>2N000005</t>
-  </si>
-  <si>
-    <t>2N000006</t>
-  </si>
-  <si>
-    <t>2N000007</t>
-  </si>
-  <si>
-    <t>2N000008</t>
-  </si>
-  <si>
-    <t>3R000001</t>
-  </si>
-  <si>
-    <t>3R000002</t>
-  </si>
-  <si>
-    <t>3R000003</t>
-  </si>
-  <si>
-    <t>3R000004</t>
-  </si>
-  <si>
-    <t>3R000005</t>
-  </si>
-  <si>
-    <t>3R000006</t>
-  </si>
-  <si>
-    <t>3R000007</t>
-  </si>
-  <si>
-    <t>3R000008</t>
-  </si>
-  <si>
-    <t>4T000001</t>
-  </si>
-  <si>
-    <t>4T000002</t>
-  </si>
-  <si>
-    <t>4T000003</t>
-  </si>
-  <si>
-    <t>4T000004</t>
-  </si>
-  <si>
-    <t>4T000005</t>
-  </si>
-  <si>
-    <t>4T000006</t>
-  </si>
-  <si>
-    <t>4T000007</t>
-  </si>
-  <si>
-    <t>4T000008</t>
   </si>
   <si>
     <t>Pass</t>
@@ -595,9 +595,9 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="sheet_name"/>
-    <tableColumn id="3" name="Date"/>
-    <tableColumn id="4" name="Author"/>
+    <tableColumn id="2" name="Author"/>
+    <tableColumn id="3" name="sheet_name"/>
+    <tableColumn id="4" name="Date"/>
     <tableColumn id="5" name="JobNo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -608,8 +608,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:I32" totalsRowShown="0">
   <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Room ID"/>
+    <tableColumn id="1" name="Room ID"/>
+    <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="Criterion 1 (% Hours Delta T &gt;= 1K)"/>
     <tableColumn id="4" name="Criterion 1 (Pass/Fail)"/>
     <tableColumn id="5" name="Criterion 2 (Max Daily Weight)"/>
@@ -626,8 +626,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:I32" totalsRowShown="0">
   <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Room ID"/>
+    <tableColumn id="1" name="Room ID"/>
+    <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="Criterion 1 (% Hours Delta T &gt;= 1K)"/>
     <tableColumn id="4" name="Criterion 1 (Pass/Fail)"/>
     <tableColumn id="5" name="Criterion 2 (Max Daily Weight)"/>
@@ -644,8 +644,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A1:I32" totalsRowShown="0">
   <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Room ID"/>
+    <tableColumn id="1" name="Room ID"/>
+    <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="Criterion 1 (% Hours Delta T &gt;= 1K)"/>
     <tableColumn id="4" name="Criterion 1 (Pass/Fail)"/>
     <tableColumn id="5" name="Criterion 2 (Max Daily Weight)"/>
@@ -684,8 +684,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:I32" totalsRowShown="0">
   <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Room ID"/>
+    <tableColumn id="1" name="Room ID"/>
+    <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="Criterion 1 (% Hours Delta T &gt;= 1K)"/>
     <tableColumn id="4" name="Criterion 1 (Pass/Fail)"/>
     <tableColumn id="5" name="Criterion 2 (Max Daily Weight)"/>
@@ -702,8 +702,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:I32" totalsRowShown="0">
   <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Room ID"/>
+    <tableColumn id="1" name="Room ID"/>
+    <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="Criterion 1 (% Hours Delta T &gt;= 1K)"/>
     <tableColumn id="4" name="Criterion 1 (Pass/Fail)"/>
     <tableColumn id="5" name="Criterion 2 (Max Daily Weight)"/>
@@ -720,8 +720,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:I32" totalsRowShown="0">
   <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Room ID"/>
+    <tableColumn id="1" name="Room ID"/>
+    <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="Criterion 1 (% Hours Delta T &gt;= 1K)"/>
     <tableColumn id="4" name="Criterion 1 (Pass/Fail)"/>
     <tableColumn id="5" name="Criterion 2 (Max Daily Weight)"/>
@@ -738,8 +738,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:I32" totalsRowShown="0">
   <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Room ID"/>
+    <tableColumn id="1" name="Room ID"/>
+    <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="Criterion 1 (% Hours Delta T &gt;= 1K)"/>
     <tableColumn id="4" name="Criterion 1 (Pass/Fail)"/>
     <tableColumn id="5" name="Criterion 2 (Max Daily Weight)"/>
@@ -756,8 +756,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:I32" totalsRowShown="0">
   <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Room ID"/>
+    <tableColumn id="1" name="Room ID"/>
+    <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="Criterion 1 (% Hours Delta T &gt;= 1K)"/>
     <tableColumn id="4" name="Criterion 1 (Pass/Fail)"/>
     <tableColumn id="5" name="Criterion 2 (Max Daily Weight)"/>
@@ -774,8 +774,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:I32" totalsRowShown="0">
   <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Room Name"/>
-    <tableColumn id="2" name="Room ID"/>
+    <tableColumn id="1" name="Room ID"/>
+    <tableColumn id="2" name="Room Name"/>
     <tableColumn id="3" name="Criterion 1 (% Hours Delta T &gt;= 1K)"/>
     <tableColumn id="4" name="Criterion 1 (Pass/Fail)"/>
     <tableColumn id="5" name="Criterion 2 (Max Daily Weight)"/>
@@ -1113,7 +1113,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>27</v>
@@ -1127,10 +1127,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>27</v>
@@ -1144,10 +1144,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
@@ -1161,10 +1161,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
@@ -1178,10 +1178,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>27</v>
@@ -1195,10 +1195,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>27</v>
@@ -1212,10 +1212,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>27</v>
@@ -1229,10 +1229,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>27</v>
@@ -1246,10 +1246,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>27</v>
@@ -1263,10 +1263,10 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>27</v>
@@ -1280,7 +1280,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Ran test model in ies
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
@@ -30,12 +30,12 @@
     <t>JobNo</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>sheet_name</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -72,7 +72,10 @@
     <t>10</t>
   </si>
   <si>
-    <t>/c/e</t>
+    <t>ngDe</t>
+  </si>
+  <si>
+    <t>20220614</t>
   </si>
   <si>
     <t>Project Information</t>
@@ -108,10 +111,7 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>20220325</t>
-  </si>
-  <si>
-    <t>jovyan</t>
+    <t>O.Hensby</t>
   </si>
   <si>
     <t>index</t>
@@ -183,7 +183,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-03-25 13:23:10.807162</t>
+    <t>2022-06-14 16:37:55.851324</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -424,7 +424,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,6 +435,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -497,7 +505,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -602,8 +610,8 @@
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="JobNo"/>
-    <tableColumn id="3" name="sheet_name"/>
-    <tableColumn id="4" name="Date"/>
+    <tableColumn id="3" name="Date"/>
+    <tableColumn id="4" name="sheet_name"/>
     <tableColumn id="5" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -624,7 +632,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -642,7 +650,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -660,7 +668,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -671,7 +679,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Information"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -682,7 +690,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Definition"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -700,7 +708,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -718,7 +726,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -736,7 +744,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -754,7 +762,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -772,7 +780,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -790,7 +798,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1122,7 +1130,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
@@ -1136,10 +1144,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
@@ -1153,10 +1161,10 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -1170,10 +1178,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
@@ -1187,10 +1195,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
@@ -1204,10 +1212,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
@@ -1221,10 +1229,10 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
@@ -1238,10 +1246,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1255,10 +1263,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>28</v>
@@ -1272,10 +1280,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -1289,7 +1297,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
@@ -6744,7 +6752,7 @@
         <v>130</v>
       </c>
       <c r="D18">
-        <v>8.140000000000001</v>
+        <v>8.14</v>
       </c>
       <c r="E18" t="s">
         <v>130</v>
@@ -6802,7 +6810,7 @@
         <v>130</v>
       </c>
       <c r="D20">
-        <v>8.039999999999999</v>
+        <v>8.04</v>
       </c>
       <c r="E20" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
Corrected output location of reports from tests
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
@@ -27,18 +27,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="131">
   <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>JobNo</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -72,10 +72,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>ngDe</t>
-  </si>
-  <si>
-    <t>20220614</t>
+    <t>jovyan</t>
   </si>
   <si>
     <t>Project Information</t>
@@ -111,7 +108,10 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>O.Hensby</t>
+    <t>20220615</t>
+  </si>
+  <si>
+    <t>/c/e</t>
   </si>
   <si>
     <t>index</t>
@@ -183,7 +183,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-06-14 16:37:55.851324</t>
+    <t>2022-06-15 10:33:09.348557</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -424,7 +424,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,14 +435,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -505,7 +497,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -609,10 +601,10 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="JobNo"/>
-    <tableColumn id="3" name="Date"/>
-    <tableColumn id="4" name="sheet_name"/>
-    <tableColumn id="5" name="Author"/>
+    <tableColumn id="2" name="Author"/>
+    <tableColumn id="3" name="sheet_name"/>
+    <tableColumn id="4" name="Date"/>
+    <tableColumn id="5" name="JobNo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -632,7 +624,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -650,7 +642,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -668,7 +660,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -679,7 +671,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Information"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -690,7 +682,7 @@
     <tableColumn id="1" name="index"/>
     <tableColumn id="2" name="Definition"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -708,7 +700,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -726,7 +718,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -744,7 +736,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -762,7 +754,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -780,7 +772,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -798,7 +790,7 @@
     <tableColumn id="8" name="Criterion 3 (Max Delta T)"/>
     <tableColumn id="9" name="TM52 (Pass/Fail)"/>
   </tableColumns>
-  <tableStyleInfo name="None" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1130,7 +1122,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
@@ -1144,10 +1136,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
@@ -1161,10 +1153,10 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -1178,10 +1170,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
@@ -1195,10 +1187,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
@@ -1212,10 +1204,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
@@ -1229,10 +1221,10 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
@@ -1246,10 +1238,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1263,10 +1255,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>28</v>
@@ -1280,10 +1272,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -1297,7 +1289,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
@@ -6752,7 +6744,7 @@
         <v>130</v>
       </c>
       <c r="D18">
-        <v>8.14</v>
+        <v>8.140000000000001</v>
       </c>
       <c r="E18" t="s">
         <v>130</v>
@@ -6810,7 +6802,7 @@
         <v>130</v>
       </c>
       <c r="D20">
-        <v>8.04</v>
+        <v>8.039999999999999</v>
       </c>
       <c r="E20" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
Updated setup. made all constants in constants file uppercase
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
@@ -27,15 +27,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="131">
   <si>
+    <t>Author</t>
+  </si>
+  <si>
     <t>JobNo</t>
   </si>
   <si>
     <t>sheet_name</t>
   </si>
   <si>
-    <t>Author</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -72,6 +72,9 @@
     <t>10</t>
   </si>
   <si>
+    <t>jovyan</t>
+  </si>
+  <si>
     <t>/c/e</t>
   </si>
   <si>
@@ -108,9 +111,6 @@
     <t>Results, Air Speed 0.8</t>
   </si>
   <si>
-    <t>jovyan</t>
-  </si>
-  <si>
     <t>20220615</t>
   </si>
   <si>
@@ -183,7 +183,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-06-15 12:25:19.129961</t>
+    <t>2022-06-15 15:57:07.449572</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -601,9 +601,9 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="JobNo"/>
-    <tableColumn id="3" name="sheet_name"/>
-    <tableColumn id="4" name="Author"/>
+    <tableColumn id="2" name="Author"/>
+    <tableColumn id="3" name="JobNo"/>
+    <tableColumn id="4" name="sheet_name"/>
     <tableColumn id="5" name="Date"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1122,7 +1122,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
@@ -1136,10 +1136,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
@@ -1153,10 +1153,10 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -1170,10 +1170,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
@@ -1187,10 +1187,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
@@ -1204,10 +1204,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
@@ -1221,10 +1221,10 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
@@ -1238,10 +1238,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1255,10 +1255,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>28</v>
@@ -1272,10 +1272,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -1289,7 +1289,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
:white_check_mark: - Fixed tests
</commit_message>
<xml_diff>
--- a/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
+++ b/tests/testmodels/TestJob1/mf_results/tm52/TM52__TestJob1.xlsx
@@ -27,15 +27,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="131">
   <si>
+    <t>sheet_name</t>
+  </si>
+  <si>
+    <t>JobNo</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>JobNo</t>
-  </si>
-  <si>
-    <t>sheet_name</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -72,43 +72,43 @@
     <t>10</t>
   </si>
   <si>
-    <t>20220615</t>
+    <t>Project Information</t>
+  </si>
+  <si>
+    <t>Criterion Definitions</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.1</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.15</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.2</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.3</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.4</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.5</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.6</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.7</t>
+  </si>
+  <si>
+    <t>Results, Air Speed 0.8</t>
   </si>
   <si>
     <t>/c/e</t>
   </si>
   <si>
-    <t>Project Information</t>
-  </si>
-  <si>
-    <t>Criterion Definitions</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.1</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.15</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.2</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.3</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.4</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.5</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.6</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.7</t>
-  </si>
-  <si>
-    <t>Results, Air Speed 0.8</t>
+    <t>20220711</t>
   </si>
   <si>
     <t>jovyan</t>
@@ -183,7 +183,7 @@
     <t>51.38</t>
   </si>
   <si>
-    <t>2022-06-15 17:01:41.020615</t>
+    <t>2022-07-11 15:53:05.032327</t>
   </si>
   <si>
     <t>2021.4.0.0</t>
@@ -601,9 +601,9 @@
   <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="index"/>
-    <tableColumn id="2" name="Date"/>
+    <tableColumn id="2" name="sheet_name"/>
     <tableColumn id="3" name="JobNo"/>
-    <tableColumn id="4" name="sheet_name"/>
+    <tableColumn id="4" name="Date"/>
     <tableColumn id="5" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1119,10 +1119,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
@@ -1133,13 +1133,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>28</v>
@@ -1150,13 +1150,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -1167,13 +1167,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
@@ -1184,13 +1184,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
@@ -1201,13 +1201,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
@@ -1218,13 +1218,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>28</v>
@@ -1235,13 +1235,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -1252,13 +1252,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>28</v>
@@ -1269,13 +1269,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -1286,10 +1286,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>

</xml_diff>